<commit_message>
Bao cao tot nghiep
</commit_message>
<xml_diff>
--- a/02. Trần Thị Diệu Linh/TCs_Build1.xlsx
+++ b/02. Trần Thị Diệu Linh/TCs_Build1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\18. Thuc tap tot nghiep\ThucTapTN_2021_2022_2\02. Trần Thị Diệu Linh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F00DAE-96FF-4662-BDFD-406449319028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B23D2F8-8F5A-4DE4-8868-99B0851931BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TR List" sheetId="1" r:id="rId1"/>
     <sheet name="TC List" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Summary TC list" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TC List'!$A$4:$J$117</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="594">
   <si>
     <t>Test Requirement List</t>
   </si>
@@ -3462,12 +3463,405 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>Build1</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Blocker</t>
+  </si>
+  <si>
+    <t>Total bugs</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Home – The banner does not match nav bar</t>
+  </si>
+  <si>
+    <t>Serverity</t>
+  </si>
+  <si>
+    <t>Register - Unable to register 2 emails in Email field at the same time</t>
+  </si>
+  <si>
+    <t>Reset Password - Unable to reset password</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Steps: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. Go to www.raillog.somee.com/Page/HomePage.cshtml#
+2. Register account with Email field contains 2 email and total length no more than 32 chars</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Observed results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>User create account successfully.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Expected results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>User cannot create account.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Attachment:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Steps: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. Go to www.raillog.somee.com/Page/HomePage.cshtml#
+2. Observe the banner on header</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Observed results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>The banner does not match nav bar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Expected results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>The banner should match nav bar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Attachment: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bug 01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Steps: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. Go to www.raillog.somee.com/Page/HomePage.cshtml#
+2. Click on FAQ tab then observe</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Observed results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nothing happens when clicking on FAQ.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Expected results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>User should create account successfully.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Attachment:</t>
+    </r>
+  </si>
+  <si>
+    <t>Timetable - Ticket price from Sài Gòn to Phan Thiết shows for all trains</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Steps: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. Go to www.raillog.somee.com/Page/TrainTimeListPage.cshtml
+2. Click on any Check Price link except first row
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Observed results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tittle table always shows: "Ticket price from Sài Gòn to Phan Thiết".</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Expected results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tittle table should match Depart and Arrive Station.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Attachment:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Steps: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. Go to www.raillog.somee.com/Account/ForgotPassword.cshtml
+2. Enter vaild email
+3. Click on Send Instructions button then observe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Observed results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Server error displays.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Expected results: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>User should reset password.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Attachment:</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3583,8 +3977,40 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3693,8 +4119,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF366092"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5DCE4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="48">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -4235,11 +4679,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="301">
+  <cellXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5037,36 +5552,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5078,15 +5565,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5104,6 +5582,25 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5113,22 +5610,89 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5701,10 +6265,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="281" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="270"/>
+      <c r="B1" s="282"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
@@ -34217,8 +34781,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA1057"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+    <sheetView showGridLines="0" topLeftCell="A98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -37563,7 +38127,7 @@
         <v>419</v>
       </c>
       <c r="F84" s="203" t="s">
-        <v>497</v>
+        <v>134</v>
       </c>
       <c r="G84" s="203" t="s">
         <v>137</v>
@@ -37735,7 +38299,7 @@
         <v>447</v>
       </c>
       <c r="F88" s="203" t="s">
-        <v>497</v>
+        <v>134</v>
       </c>
       <c r="G88" s="210" t="s">
         <v>137</v>
@@ -37821,7 +38385,7 @@
         <v>448</v>
       </c>
       <c r="F90" s="203" t="s">
-        <v>497</v>
+        <v>134</v>
       </c>
       <c r="G90" s="210" t="s">
         <v>137</v>
@@ -37952,7 +38516,7 @@
         <v>424</v>
       </c>
       <c r="F93" s="203" t="s">
-        <v>497</v>
+        <v>134</v>
       </c>
       <c r="G93" s="210" t="s">
         <v>137</v>
@@ -37997,7 +38561,7 @@
         <v>461</v>
       </c>
       <c r="F94" s="203" t="s">
-        <v>497</v>
+        <v>134</v>
       </c>
       <c r="G94" s="210" t="s">
         <v>137</v>
@@ -38128,7 +38692,7 @@
         <v>424</v>
       </c>
       <c r="F97" s="203" t="s">
-        <v>497</v>
+        <v>134</v>
       </c>
       <c r="G97" s="210" t="s">
         <v>137</v>
@@ -38171,7 +38735,7 @@
         <v>424</v>
       </c>
       <c r="F98" s="203" t="s">
-        <v>497</v>
+        <v>134</v>
       </c>
       <c r="G98" s="210" t="s">
         <v>137</v>
@@ -66237,17 +66801,17 @@
     </filterColumn>
   </autoFilter>
   <phoneticPr fontId="19" type="noConversion"/>
-  <conditionalFormatting sqref="F119:F1057 F111:F117 F74:F78 F8:G72 F80:F109">
+  <conditionalFormatting sqref="F119:F1057 F111:F117 F74:F78 F8:G72 F80:F83 F85:F87 F89 F91:F92 F95:F96 F99:F109">
     <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F119:F1057 F111:F117 F74:F78 F8:G72 F80:F109">
+  <conditionalFormatting sqref="F119:F1057 F111:F117 F74:F78 F8:G72 F80:F83 F85:F87 F89 F91:F92 F95:F96 F99:F109">
     <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F119:F1057 F111:F117 F74:F78 F8:G72 F80:F109">
+  <conditionalFormatting sqref="F119:F1057 F111:F117 F74:F78 F8:G72 F80:F83 F85:F87 F89 F91:F92 F95:F96 F99:F109">
     <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
@@ -66297,17 +66861,17 @@
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F79">
+  <conditionalFormatting sqref="F79 F84 F88 F90 F93:F94 F97:F98">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F79">
+  <conditionalFormatting sqref="F79 F84 F88 F90 F93:F94 F97:F98">
     <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F79">
+  <conditionalFormatting sqref="F79 F84 F88 F90 F93:F94 F97:F98">
     <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
@@ -66461,7 +67025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E7A849-9089-4B3D-BF51-444C57119794}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A43" sqref="A43:F56"/>
     </sheetView>
   </sheetViews>
@@ -66478,22 +67042,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="292" t="s">
         <v>525</v>
       </c>
-      <c r="B1" s="284" t="s">
+      <c r="B1" s="295" t="s">
         <v>570</v>
       </c>
-      <c r="C1" s="285"/>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="283"/>
+      <c r="C1" s="296"/>
+      <c r="D1" s="296"/>
+      <c r="E1" s="296"/>
+      <c r="F1" s="296"/>
+      <c r="G1" s="297"/>
+      <c r="H1" s="273"/>
     </row>
     <row r="2" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A2" s="278"/>
-      <c r="B2" s="277" t="s">
+      <c r="A2" s="293"/>
+      <c r="B2" s="292" t="s">
         <v>564</v>
       </c>
       <c r="C2" s="260" t="s">
@@ -66511,54 +67075,54 @@
       <c r="G2" s="260" t="s">
         <v>557</v>
       </c>
-      <c r="H2" s="283"/>
+      <c r="H2" s="273"/>
     </row>
     <row r="3" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A3" s="278"/>
-      <c r="B3" s="278"/>
-      <c r="C3" s="281">
+      <c r="A3" s="293"/>
+      <c r="B3" s="293"/>
+      <c r="C3" s="271">
         <v>44632</v>
       </c>
-      <c r="D3" s="281">
+      <c r="D3" s="271">
         <v>44639</v>
       </c>
-      <c r="E3" s="281">
+      <c r="E3" s="271">
         <v>44646</v>
       </c>
-      <c r="F3" s="281">
+      <c r="F3" s="271">
         <v>44647</v>
       </c>
-      <c r="G3" s="282">
+      <c r="G3" s="272">
         <v>44682</v>
       </c>
-      <c r="H3" s="283" t="s">
+      <c r="H3" s="273" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="54.75" customHeight="1">
-      <c r="A4" s="279"/>
-      <c r="B4" s="279"/>
-      <c r="C4" s="282">
+      <c r="A4" s="294"/>
+      <c r="B4" s="294"/>
+      <c r="C4" s="272">
         <v>44633</v>
       </c>
-      <c r="D4" s="282">
+      <c r="D4" s="272">
         <v>44639</v>
       </c>
-      <c r="E4" s="282">
+      <c r="E4" s="272">
         <v>44646</v>
       </c>
-      <c r="F4" s="282">
+      <c r="F4" s="272">
         <v>44682</v>
       </c>
-      <c r="G4" s="282">
+      <c r="G4" s="272">
         <v>44682</v>
       </c>
-      <c r="H4" s="283" t="s">
+      <c r="H4" s="273" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A5" s="287" t="s">
+      <c r="A5" s="274" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="258" t="s">
@@ -66579,10 +67143,10 @@
       <c r="G5" s="258">
         <v>0.02</v>
       </c>
-      <c r="H5" s="283"/>
+      <c r="H5" s="273"/>
     </row>
     <row r="6" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A6" s="287" t="s">
+      <c r="A6" s="274" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="258" t="s">
@@ -66603,10 +67167,10 @@
       <c r="G6" s="258">
         <v>0.05</v>
       </c>
-      <c r="H6" s="283"/>
+      <c r="H6" s="273"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="287" t="s">
+      <c r="A7" s="274" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="258" t="s">
@@ -66627,10 +67191,10 @@
       <c r="G7" s="258">
         <v>0.02</v>
       </c>
-      <c r="H7" s="283"/>
+      <c r="H7" s="273"/>
     </row>
     <row r="8" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A8" s="287" t="s">
+      <c r="A8" s="274" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="258" t="s">
@@ -66651,10 +67215,10 @@
       <c r="G8" s="258">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H8" s="283"/>
+      <c r="H8" s="273"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A9" s="287" t="s">
+      <c r="A9" s="274" t="s">
         <v>61</v>
       </c>
       <c r="B9" s="258" t="s">
@@ -66675,10 +67239,10 @@
       <c r="G9" s="258">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H9" s="283"/>
+      <c r="H9" s="273"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="287" t="s">
+      <c r="A10" s="274" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="258" t="s">
@@ -66699,10 +67263,10 @@
       <c r="G10" s="258">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H10" s="283"/>
+      <c r="H10" s="273"/>
     </row>
     <row r="11" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A11" s="287" t="s">
+      <c r="A11" s="274" t="s">
         <v>77</v>
       </c>
       <c r="B11" s="258" t="s">
@@ -66723,10 +67287,10 @@
       <c r="G11" s="258">
         <v>0.01</v>
       </c>
-      <c r="H11" s="283"/>
+      <c r="H11" s="273"/>
     </row>
     <row r="12" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A12" s="287" t="s">
+      <c r="A12" s="274" t="s">
         <v>85</v>
       </c>
       <c r="B12" s="258" t="s">
@@ -66747,10 +67311,10 @@
       <c r="G12" s="258">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H12" s="283"/>
+      <c r="H12" s="273"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A13" s="287" t="s">
+      <c r="A13" s="274" t="s">
         <v>569</v>
       </c>
       <c r="B13" s="258" t="s">
@@ -66771,10 +67335,10 @@
       <c r="G13" s="258">
         <v>0.35</v>
       </c>
-      <c r="H13" s="283"/>
+      <c r="H13" s="273"/>
     </row>
     <row r="14" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A14" s="287" t="s">
+      <c r="A14" s="274" t="s">
         <v>104</v>
       </c>
       <c r="B14" s="258" t="s">
@@ -66795,10 +67359,10 @@
       <c r="G14" s="258">
         <v>0.03</v>
       </c>
-      <c r="H14" s="283"/>
+      <c r="H14" s="273"/>
     </row>
     <row r="15" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A15" s="287" t="s">
+      <c r="A15" s="274" t="s">
         <v>349</v>
       </c>
       <c r="B15" s="258" t="s">
@@ -66819,10 +67383,10 @@
       <c r="G15" s="258">
         <v>0.01</v>
       </c>
-      <c r="H15" s="283"/>
+      <c r="H15" s="273"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A16" s="287" t="s">
+      <c r="A16" s="274" t="s">
         <v>115</v>
       </c>
       <c r="B16" s="258" t="s">
@@ -66843,13 +67407,13 @@
       <c r="G16" s="258">
         <v>0.04</v>
       </c>
-      <c r="H16" s="283"/>
+      <c r="H16" s="273"/>
     </row>
     <row r="17" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A17" s="274" t="s">
+      <c r="A17" s="289" t="s">
         <v>526</v>
       </c>
-      <c r="B17" s="276"/>
+      <c r="B17" s="291"/>
       <c r="C17" s="258">
         <f>SUM(C5:C16)</f>
         <v>12.73</v>
@@ -66870,26 +67434,26 @@
         <f>SUM(G5:G16)</f>
         <v>0.55800000000000005</v>
       </c>
-      <c r="H17" s="283"/>
+      <c r="H17" s="273"/>
     </row>
     <row r="21" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="22" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A22" s="292" t="s">
+      <c r="A22" s="286" t="s">
         <v>525</v>
       </c>
-      <c r="B22" s="296" t="s">
+      <c r="B22" s="283" t="s">
         <v>570</v>
       </c>
-      <c r="C22" s="295"/>
-      <c r="D22" s="295"/>
-      <c r="E22" s="295"/>
-      <c r="F22" s="295"/>
-      <c r="G22" s="297"/>
-      <c r="H22" s="280"/>
+      <c r="C22" s="284"/>
+      <c r="D22" s="284"/>
+      <c r="E22" s="284"/>
+      <c r="F22" s="284"/>
+      <c r="G22" s="285"/>
+      <c r="H22" s="270"/>
     </row>
     <row r="23" spans="1:9" ht="33.75" thickBot="1">
-      <c r="A23" s="293"/>
-      <c r="B23" s="292" t="s">
+      <c r="A23" s="287"/>
+      <c r="B23" s="286" t="s">
         <v>564</v>
       </c>
       <c r="C23" s="258" t="s">
@@ -66907,56 +67471,56 @@
       <c r="G23" s="258" t="s">
         <v>557</v>
       </c>
-      <c r="H23" s="280"/>
+      <c r="H23" s="270"/>
     </row>
     <row r="24" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A24" s="293"/>
-      <c r="B24" s="293"/>
-      <c r="C24" s="288">
+      <c r="A24" s="287"/>
+      <c r="B24" s="287"/>
+      <c r="C24" s="275">
         <v>44632</v>
       </c>
-      <c r="D24" s="288">
+      <c r="D24" s="275">
         <v>44639</v>
       </c>
-      <c r="E24" s="288">
+      <c r="E24" s="275">
         <v>44646</v>
       </c>
-      <c r="F24" s="288">
+      <c r="F24" s="275">
         <v>44647</v>
       </c>
-      <c r="G24" s="289">
+      <c r="G24" s="276">
         <v>44682</v>
       </c>
-      <c r="H24" s="283" t="s">
+      <c r="H24" s="273" t="s">
         <v>573</v>
       </c>
-      <c r="I24" s="289"/>
+      <c r="I24" s="276"/>
     </row>
     <row r="25" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A25" s="294"/>
-      <c r="B25" s="294"/>
-      <c r="C25" s="290">
+      <c r="A25" s="288"/>
+      <c r="B25" s="288"/>
+      <c r="C25" s="277">
         <v>44633</v>
       </c>
-      <c r="D25" s="290">
+      <c r="D25" s="277">
         <v>44639</v>
       </c>
-      <c r="E25" s="290">
+      <c r="E25" s="277">
         <v>44646</v>
       </c>
-      <c r="F25" s="290">
+      <c r="F25" s="277">
         <v>44682</v>
       </c>
-      <c r="G25" s="290">
+      <c r="G25" s="277">
         <v>44682</v>
       </c>
-      <c r="H25" s="283" t="s">
+      <c r="H25" s="273" t="s">
         <v>574</v>
       </c>
-      <c r="I25" s="290"/>
+      <c r="I25" s="277"/>
     </row>
     <row r="26" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A26" s="291" t="s">
+      <c r="A26" s="278" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="258" t="s">
@@ -66977,10 +67541,10 @@
       <c r="G26" s="258">
         <v>0.02</v>
       </c>
-      <c r="H26" s="280"/>
+      <c r="H26" s="270"/>
     </row>
     <row r="27" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A27" s="291" t="s">
+      <c r="A27" s="278" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="258" t="s">
@@ -67001,10 +67565,10 @@
       <c r="G27" s="258">
         <v>0.05</v>
       </c>
-      <c r="H27" s="280"/>
+      <c r="H27" s="270"/>
     </row>
     <row r="28" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A28" s="291" t="s">
+      <c r="A28" s="278" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="258" t="s">
@@ -67025,10 +67589,10 @@
       <c r="G28" s="258">
         <v>0.02</v>
       </c>
-      <c r="H28" s="280"/>
+      <c r="H28" s="270"/>
     </row>
     <row r="29" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A29" s="291" t="s">
+      <c r="A29" s="278" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="258" t="s">
@@ -67049,10 +67613,10 @@
       <c r="G29" s="258">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H29" s="280"/>
+      <c r="H29" s="270"/>
     </row>
     <row r="30" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A30" s="291" t="s">
+      <c r="A30" s="278" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="258" t="s">
@@ -67073,10 +67637,10 @@
       <c r="G30" s="258">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H30" s="280"/>
+      <c r="H30" s="270"/>
     </row>
     <row r="31" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A31" s="291" t="s">
+      <c r="A31" s="278" t="s">
         <v>66</v>
       </c>
       <c r="B31" s="258" t="s">
@@ -67097,10 +67661,10 @@
       <c r="G31" s="258">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H31" s="280"/>
+      <c r="H31" s="270"/>
     </row>
     <row r="32" spans="1:9" ht="17.25" thickBot="1">
-      <c r="A32" s="291" t="s">
+      <c r="A32" s="278" t="s">
         <v>77</v>
       </c>
       <c r="B32" s="258" t="s">
@@ -67121,10 +67685,10 @@
       <c r="G32" s="258">
         <v>0.01</v>
       </c>
-      <c r="H32" s="280"/>
+      <c r="H32" s="270"/>
     </row>
     <row r="33" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A33" s="291" t="s">
+      <c r="A33" s="278" t="s">
         <v>85</v>
       </c>
       <c r="B33" s="258" t="s">
@@ -67145,10 +67709,10 @@
       <c r="G33" s="258">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H33" s="280"/>
+      <c r="H33" s="270"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A34" s="291" t="s">
+      <c r="A34" s="278" t="s">
         <v>569</v>
       </c>
       <c r="B34" s="258" t="s">
@@ -67169,10 +67733,10 @@
       <c r="G34" s="258">
         <v>0.35</v>
       </c>
-      <c r="H34" s="280"/>
+      <c r="H34" s="270"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A35" s="291" t="s">
+      <c r="A35" s="278" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="258" t="s">
@@ -67193,10 +67757,10 @@
       <c r="G35" s="258">
         <v>0.03</v>
       </c>
-      <c r="H35" s="280"/>
+      <c r="H35" s="270"/>
     </row>
     <row r="36" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A36" s="291" t="s">
+      <c r="A36" s="278" t="s">
         <v>349</v>
       </c>
       <c r="B36" s="258" t="s">
@@ -67217,10 +67781,10 @@
       <c r="G36" s="258">
         <v>0.01</v>
       </c>
-      <c r="H36" s="280"/>
+      <c r="H36" s="270"/>
     </row>
     <row r="37" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A37" s="291" t="s">
+      <c r="A37" s="278" t="s">
         <v>115</v>
       </c>
       <c r="B37" s="258" t="s">
@@ -67241,13 +67805,13 @@
       <c r="G37" s="258">
         <v>0.04</v>
       </c>
-      <c r="H37" s="280"/>
+      <c r="H37" s="270"/>
     </row>
     <row r="38" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A38" s="274" t="s">
+      <c r="A38" s="289" t="s">
         <v>526</v>
       </c>
-      <c r="B38" s="298"/>
+      <c r="B38" s="290"/>
       <c r="C38" s="258">
         <v>12.73</v>
       </c>
@@ -67263,31 +67827,31 @@
       <c r="G38" s="258">
         <v>0.55800000000000005</v>
       </c>
-      <c r="H38" s="280"/>
+      <c r="H38" s="270"/>
     </row>
     <row r="42" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:8" ht="33.75" thickBot="1">
-      <c r="A43" s="299" t="s">
+      <c r="A43" s="279" t="s">
         <v>525</v>
       </c>
-      <c r="B43" s="300" t="s">
+      <c r="B43" s="280" t="s">
         <v>575</v>
       </c>
-      <c r="C43" s="300" t="s">
+      <c r="C43" s="280" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="300" t="s">
+      <c r="D43" s="280" t="s">
         <v>134</v>
       </c>
-      <c r="E43" s="300" t="s">
+      <c r="E43" s="280" t="s">
         <v>497</v>
       </c>
-      <c r="F43" s="300" t="s">
+      <c r="F43" s="280" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A44" s="287" t="s">
+      <c r="A44" s="274" t="s">
         <v>6</v>
       </c>
       <c r="B44" s="258">
@@ -67307,7 +67871,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A45" s="287" t="s">
+      <c r="A45" s="274" t="s">
         <v>20</v>
       </c>
       <c r="B45" s="258">
@@ -67327,7 +67891,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A46" s="287" t="s">
+      <c r="A46" s="274" t="s">
         <v>27</v>
       </c>
       <c r="B46" s="258">
@@ -67347,7 +67911,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A47" s="287" t="s">
+      <c r="A47" s="274" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="258">
@@ -67367,7 +67931,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A48" s="287" t="s">
+      <c r="A48" s="274" t="s">
         <v>61</v>
       </c>
       <c r="B48" s="258">
@@ -67387,7 +67951,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A49" s="287" t="s">
+      <c r="A49" s="274" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="258">
@@ -67407,7 +67971,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A50" s="287" t="s">
+      <c r="A50" s="274" t="s">
         <v>77</v>
       </c>
       <c r="B50" s="258">
@@ -67427,7 +67991,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A51" s="287" t="s">
+      <c r="A51" s="274" t="s">
         <v>85</v>
       </c>
       <c r="B51" s="258">
@@ -67447,7 +68011,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A52" s="287" t="s">
+      <c r="A52" s="274" t="s">
         <v>569</v>
       </c>
       <c r="B52" s="258">
@@ -67467,7 +68031,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A53" s="287" t="s">
+      <c r="A53" s="274" t="s">
         <v>104</v>
       </c>
       <c r="B53" s="258">
@@ -67487,7 +68051,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A54" s="287" t="s">
+      <c r="A54" s="274" t="s">
         <v>349</v>
       </c>
       <c r="B54" s="258">
@@ -67507,7 +68071,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A55" s="287" t="s">
+      <c r="A55" s="274" t="s">
         <v>115</v>
       </c>
       <c r="B55" s="258">
@@ -67527,7 +68091,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A56" s="287" t="s">
+      <c r="A56" s="274" t="s">
         <v>526</v>
       </c>
       <c r="B56" s="258">
@@ -67564,714 +68128,1195 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A98A753-3A09-4404-9B44-374DF1BDDDD2}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45:G45"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="1" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27.75" customHeight="1">
-      <c r="A1" s="271" t="s">
+    <row r="1" spans="1:11" ht="27.75" customHeight="1">
+      <c r="A1" s="298" t="s">
         <v>523</v>
       </c>
-      <c r="B1" s="234" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="234" t="s">
         <v>525</v>
       </c>
-      <c r="C1" s="234" t="s">
+      <c r="D1" s="234" t="s">
         <v>524</v>
       </c>
-      <c r="D1" s="236" t="s">
+      <c r="E1" s="236" t="s">
         <v>529</v>
       </c>
-      <c r="E1" s="235" t="s">
+      <c r="F1" s="235" t="s">
         <v>527</v>
       </c>
-      <c r="F1" s="235" t="s">
+      <c r="G1" s="235" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="271"/>
-      <c r="B2" s="232" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="298"/>
+      <c r="B2" s="269"/>
+      <c r="C2" s="232" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
-      </c>
-      <c r="E2" s="238">
-        <v>44660</v>
       </c>
       <c r="F2" s="238">
         <v>44660</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="271"/>
-      <c r="B3" s="232" t="s">
+      <c r="G2" s="238">
+        <v>44660</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="298"/>
+      <c r="B3" s="269"/>
+      <c r="C3" s="232" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>23</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>92</v>
-      </c>
-      <c r="E3" s="238">
-        <v>44660</v>
       </c>
       <c r="F3" s="238">
         <v>44660</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="271"/>
-      <c r="B4" s="233" t="s">
+      <c r="G3" s="238">
+        <v>44660</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="298"/>
+      <c r="B4" s="269"/>
+      <c r="C4" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>32</v>
-      </c>
-      <c r="E4" s="238">
-        <v>44660</v>
       </c>
       <c r="F4" s="238">
         <v>44660</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="271"/>
-      <c r="B5" s="232" t="s">
+      <c r="G4" s="238">
+        <v>44660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="298"/>
+      <c r="B5" s="269"/>
+      <c r="C5" s="232" t="s">
         <v>43</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>6</v>
-      </c>
-      <c r="E5" s="238">
-        <v>44660</v>
       </c>
       <c r="F5" s="238">
         <v>44660</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="271"/>
-      <c r="B6" s="232" t="s">
+      <c r="G5" s="238">
+        <v>44660</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="298"/>
+      <c r="B6" s="269"/>
+      <c r="C6" s="232" t="s">
         <v>61</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>6</v>
-      </c>
-      <c r="E6" s="238">
-        <v>44661</v>
       </c>
       <c r="F6" s="238">
         <v>44661</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="271"/>
-      <c r="B7" s="232" t="s">
+      <c r="G6" s="238">
+        <v>44661</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="298"/>
+      <c r="B7" s="269"/>
+      <c r="C7" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>7</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>28</v>
-      </c>
-      <c r="E7" s="238">
-        <v>44661</v>
       </c>
       <c r="F7" s="238">
         <v>44661</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="271"/>
-      <c r="B8" s="232" t="s">
+      <c r="G7" s="238">
+        <v>44661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="298"/>
+      <c r="B8" s="269"/>
+      <c r="C8" s="232" t="s">
         <v>77</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>16</v>
-      </c>
-      <c r="E8" s="238">
-        <v>44661</v>
       </c>
       <c r="F8" s="238">
         <v>44661</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="271"/>
-      <c r="B9" s="232" t="s">
+      <c r="G8" s="238">
+        <v>44661</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="298"/>
+      <c r="B9" s="269"/>
+      <c r="C9" s="232" t="s">
         <v>85</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>42</v>
-      </c>
-      <c r="E9" s="238">
-        <v>44661</v>
       </c>
       <c r="F9" s="238">
         <v>44661</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="271"/>
-      <c r="B10" s="232" t="s">
+      <c r="G9" s="238">
+        <v>44661</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="298"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="232" t="s">
         <v>93</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="271"/>
-      <c r="B11" s="232" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" s="298"/>
+      <c r="B11" s="269"/>
+      <c r="C11" s="232" t="s">
         <v>104</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="271"/>
-      <c r="B12" s="232" t="s">
+    <row r="12" spans="1:11">
+      <c r="A12" s="298"/>
+      <c r="B12" s="269"/>
+      <c r="C12" s="232" t="s">
         <v>349</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="271"/>
-      <c r="B13" s="237" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" s="298"/>
+      <c r="B13" s="269"/>
+      <c r="C13" s="237" t="s">
         <v>115</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>526</v>
       </c>
-      <c r="C14">
-        <f>SUM(C2:C13)</f>
+      <c r="D14">
+        <f>SUM(D2:D13)</f>
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="16.5">
+    <row r="16" spans="1:11" ht="16.5">
       <c r="A16" s="265" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="260" t="s">
+      <c r="B16" s="265"/>
+      <c r="C16" s="260" t="s">
         <v>550</v>
       </c>
-      <c r="C16" s="260" t="s">
+      <c r="D16" s="260" t="s">
         <v>551</v>
       </c>
-      <c r="D16" s="260" t="s">
+      <c r="E16" s="260" t="s">
         <v>552</v>
       </c>
-      <c r="E16" s="261" t="s">
+      <c r="F16" s="261" t="s">
         <v>558</v>
       </c>
-      <c r="G16" s="264" t="s">
+      <c r="H16" s="264" t="s">
         <v>560</v>
       </c>
-      <c r="H16" s="264" t="s">
+      <c r="I16" s="264" t="s">
         <v>559</v>
       </c>
-      <c r="I16" s="264" t="s">
+      <c r="J16" s="264" t="s">
         <v>562</v>
       </c>
-      <c r="J16" s="264" t="s">
+      <c r="K16" s="264" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="33">
+    <row r="17" spans="1:11" ht="33">
       <c r="A17" s="262" t="s">
         <v>553</v>
       </c>
-      <c r="B17" s="260">
+      <c r="B17" s="262"/>
+      <c r="C17" s="260">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C17" s="260">
+      <c r="D17" s="260">
         <v>0.05</v>
       </c>
-      <c r="D17" s="260">
+      <c r="E17" s="260">
         <v>0.1</v>
       </c>
-      <c r="E17" s="263">
-        <f>ROUND(((B17+4*C17+D17)/6),2)</f>
+      <c r="F17" s="263">
+        <f>ROUND(((C17+4*D17+E17)/6),2)</f>
         <v>0.06</v>
       </c>
-      <c r="F17" s="265">
-        <f>(G17*H17)/60</f>
+      <c r="G17" s="265">
+        <f>(H17*I17)/60</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G17" s="264">
+      <c r="H17" s="264">
         <v>1.5</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>1</v>
-      </c>
-      <c r="I17">
-        <v>5</v>
       </c>
       <c r="J17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="33">
+      <c r="K17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="33">
       <c r="A18" s="262" t="s">
         <v>554</v>
       </c>
-      <c r="B18" s="260">
+      <c r="B18" s="262"/>
+      <c r="C18" s="260">
         <v>0.05</v>
       </c>
-      <c r="C18" s="260">
+      <c r="D18" s="260">
         <v>0.03</v>
       </c>
-      <c r="D18" s="260">
+      <c r="E18" s="260">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E18" s="263">
-        <f t="shared" ref="E18:E21" si="0">ROUND(((B18+4*C18+D18)/6),2)</f>
+      <c r="F18" s="263">
+        <f t="shared" ref="F18:F21" si="0">ROUND(((C18+4*D18+E18)/6),2)</f>
         <v>0.04</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="49.5">
+    <row r="19" spans="1:11" ht="49.5">
       <c r="A19" s="262" t="s">
         <v>555</v>
       </c>
-      <c r="B19" s="260">
+      <c r="B19" s="262"/>
+      <c r="C19" s="260">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="C19" s="260">
+      <c r="D19" s="260">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="D19" s="260">
+      <c r="E19" s="260">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E19" s="263">
-        <f>ROUND(((B19+4*C19+D19)/6),2)</f>
+      <c r="F19" s="263">
+        <f>ROUND(((C19+4*D19+E19)/6),2)</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="33">
+    <row r="20" spans="1:11" ht="33">
       <c r="A20" s="262" t="s">
         <v>556</v>
       </c>
-      <c r="B20" s="260">
+      <c r="B20" s="262"/>
+      <c r="C20" s="260">
         <v>0.17</v>
       </c>
-      <c r="C20" s="260">
+      <c r="D20" s="260">
         <v>0.13</v>
       </c>
-      <c r="D20" s="260">
+      <c r="E20" s="260">
         <v>0.25</v>
       </c>
-      <c r="E20" s="263">
+      <c r="F20" s="263">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="49.5">
+    <row r="21" spans="1:11" ht="49.5">
       <c r="A21" s="262" t="s">
         <v>557</v>
       </c>
-      <c r="B21" s="260">
+      <c r="B21" s="262"/>
+      <c r="C21" s="260">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C21" s="260">
+      <c r="D21" s="260">
         <v>0.13</v>
       </c>
-      <c r="D21" s="260">
+      <c r="E21" s="260">
         <v>0.25</v>
       </c>
-      <c r="E21" s="263">
+      <c r="F21" s="263">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16.5">
+    <row r="22" spans="1:11" ht="16.5">
       <c r="A22" s="259"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.5" thickBot="1"/>
-    <row r="31" spans="1:10" ht="17.25" thickBot="1">
-      <c r="A31" s="272" t="s">
+      <c r="B22" s="307"/>
+    </row>
+    <row r="30" spans="1:11" ht="13.5" thickBot="1"/>
+    <row r="31" spans="1:11" ht="17.25" thickBot="1">
+      <c r="A31" s="299" t="s">
         <v>525</v>
       </c>
-      <c r="B31" s="274" t="s">
+      <c r="B31" s="308"/>
+      <c r="C31" s="289" t="s">
         <v>563</v>
       </c>
-      <c r="C31" s="275"/>
-      <c r="D31" s="275"/>
-      <c r="E31" s="275"/>
-      <c r="F31" s="275"/>
-      <c r="G31" s="276"/>
-    </row>
-    <row r="32" spans="1:10" ht="66.75" thickBot="1">
-      <c r="A32" s="273"/>
-      <c r="B32" s="258" t="s">
+      <c r="D31" s="301"/>
+      <c r="E31" s="301"/>
+      <c r="F31" s="301"/>
+      <c r="G31" s="301"/>
+      <c r="H31" s="291"/>
+    </row>
+    <row r="32" spans="1:11" ht="66.75" thickBot="1">
+      <c r="A32" s="300"/>
+      <c r="B32" s="268"/>
+      <c r="C32" s="258" t="s">
         <v>564</v>
       </c>
-      <c r="C32" s="258" t="s">
+      <c r="D32" s="258" t="s">
         <v>565</v>
       </c>
-      <c r="D32" s="266" t="s">
+      <c r="E32" s="266" t="s">
         <v>566</v>
       </c>
-      <c r="E32" s="258" t="s">
+      <c r="F32" s="258" t="s">
         <v>555</v>
       </c>
-      <c r="F32" s="258" t="s">
+      <c r="G32" s="258" t="s">
         <v>556</v>
       </c>
-      <c r="G32" s="258" t="s">
+      <c r="H32" s="258" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17.25" thickBot="1">
+    <row r="33" spans="1:8" ht="17.25" thickBot="1">
       <c r="A33" s="267" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="258" t="s">
+      <c r="B33" s="268"/>
+      <c r="C33" s="258" t="s">
         <v>567</v>
       </c>
-      <c r="C33" s="258">
+      <c r="D33" s="258">
         <v>0.21</v>
       </c>
-      <c r="D33" s="258">
+      <c r="E33" s="258">
         <v>0.13</v>
       </c>
-      <c r="E33" s="258">
+      <c r="F33" s="258">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="F33" s="258">
+      <c r="G33" s="258">
         <v>0.25</v>
       </c>
-      <c r="G33" s="258">
+      <c r="H33" s="258">
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.25" thickBot="1">
+    <row r="34" spans="1:8" ht="17.25" thickBot="1">
       <c r="A34" s="267" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="258" t="s">
+      <c r="B34" s="268"/>
+      <c r="C34" s="258" t="s">
         <v>568</v>
       </c>
-      <c r="C34" s="258">
+      <c r="D34" s="258">
         <v>1.53</v>
       </c>
-      <c r="D34" s="258">
+      <c r="E34" s="258">
         <v>1.72</v>
       </c>
-      <c r="E34" s="258">
+      <c r="F34" s="258">
         <v>1.41</v>
       </c>
-      <c r="F34" s="258">
+      <c r="G34" s="258">
         <v>3.66</v>
       </c>
-      <c r="G34" s="258">
+      <c r="H34" s="258">
         <v>0.39</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.25" thickBot="1">
+    <row r="35" spans="1:8" ht="17.25" thickBot="1">
       <c r="A35" s="267" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="258" t="s">
+      <c r="B35" s="268"/>
+      <c r="C35" s="258" t="s">
         <v>568</v>
       </c>
-      <c r="C35" s="258">
+      <c r="D35" s="258">
         <v>0.7</v>
       </c>
-      <c r="D35" s="258">
+      <c r="E35" s="258">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E35" s="258">
+      <c r="F35" s="258">
         <v>0.23</v>
       </c>
-      <c r="F35" s="258">
+      <c r="G35" s="258">
         <v>1.29</v>
       </c>
-      <c r="G35" s="258">
+      <c r="H35" s="258">
         <v>0.13</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17.25" thickBot="1">
+    <row r="36" spans="1:8" ht="17.25" thickBot="1">
       <c r="A36" s="267" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="258" t="s">
+      <c r="B36" s="268"/>
+      <c r="C36" s="258" t="s">
         <v>567</v>
       </c>
-      <c r="C36" s="258">
+      <c r="D36" s="258">
         <v>0.21</v>
       </c>
-      <c r="D36" s="258">
+      <c r="E36" s="258">
         <v>0.18</v>
       </c>
-      <c r="E36" s="258">
+      <c r="F36" s="258">
         <v>0.05</v>
       </c>
-      <c r="F36" s="258">
+      <c r="G36" s="258">
         <v>0.11</v>
       </c>
-      <c r="G36" s="258">
+      <c r="H36" s="258">
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.25" thickBot="1">
+    <row r="37" spans="1:8" ht="17.25" thickBot="1">
       <c r="A37" s="267" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="258" t="s">
+      <c r="B37" s="268"/>
+      <c r="C37" s="258" t="s">
         <v>567</v>
       </c>
-      <c r="C37" s="258">
+      <c r="D37" s="258">
         <v>0.21</v>
       </c>
-      <c r="D37" s="258">
+      <c r="E37" s="258">
         <v>0.18</v>
       </c>
-      <c r="E37" s="258">
+      <c r="F37" s="258">
         <v>0.03</v>
       </c>
-      <c r="F37" s="258">
+      <c r="G37" s="258">
         <v>0.19</v>
       </c>
-      <c r="G37" s="258">
+      <c r="H37" s="258">
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="33.75" thickBot="1">
+    <row r="38" spans="1:8" ht="33.75" thickBot="1">
       <c r="A38" s="267" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="258" t="s">
+      <c r="B38" s="268"/>
+      <c r="C38" s="258" t="s">
         <v>568</v>
-      </c>
-      <c r="C38" s="258">
-        <v>0.47</v>
       </c>
       <c r="D38" s="258">
         <v>0.47</v>
       </c>
       <c r="E38" s="258">
+        <v>0.47</v>
+      </c>
+      <c r="F38" s="258">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F38" s="258">
+      <c r="G38" s="258">
         <v>0.23</v>
       </c>
-      <c r="G38" s="258">
+      <c r="H38" s="258">
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="33.75" thickBot="1">
+    <row r="39" spans="1:8" ht="33.75" thickBot="1">
       <c r="A39" s="267" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="258" t="s">
+      <c r="B39" s="268"/>
+      <c r="C39" s="258" t="s">
         <v>568</v>
       </c>
-      <c r="C39" s="258">
+      <c r="D39" s="258">
         <v>0.31</v>
       </c>
-      <c r="D39" s="258">
+      <c r="E39" s="258">
         <v>0.17</v>
       </c>
-      <c r="E39" s="258">
+      <c r="F39" s="258">
         <v>0.04</v>
       </c>
-      <c r="F39" s="258">
+      <c r="G39" s="258">
         <v>0.63</v>
       </c>
-      <c r="G39" s="258">
+      <c r="H39" s="258">
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="33.75" thickBot="1">
+    <row r="40" spans="1:8" ht="33.75" thickBot="1">
       <c r="A40" s="267" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="258" t="s">
+      <c r="B40" s="268"/>
+      <c r="C40" s="258" t="s">
         <v>568</v>
       </c>
-      <c r="C40" s="258">
+      <c r="D40" s="258">
         <v>1.1100000000000001</v>
       </c>
-      <c r="D40" s="258">
+      <c r="E40" s="258">
         <v>0.53</v>
       </c>
-      <c r="E40" s="258">
+      <c r="F40" s="258">
         <v>0.18</v>
       </c>
-      <c r="F40" s="258">
+      <c r="G40" s="258">
         <v>0.63</v>
       </c>
-      <c r="G40" s="258">
+      <c r="H40" s="258">
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="33.75" thickBot="1">
+    <row r="41" spans="1:8" ht="33.75" thickBot="1">
       <c r="A41" s="267" t="s">
         <v>569</v>
       </c>
-      <c r="B41" s="258" t="s">
+      <c r="B41" s="268"/>
+      <c r="C41" s="258" t="s">
         <v>568</v>
       </c>
-      <c r="C41" s="258">
+      <c r="D41" s="258">
         <v>2.34</v>
       </c>
-      <c r="D41" s="258">
+      <c r="E41" s="258">
         <v>1.24</v>
       </c>
-      <c r="E41" s="268">
+      <c r="F41" s="268">
         <v>0.37</v>
       </c>
-      <c r="F41" s="258">
+      <c r="G41" s="258">
         <v>6.23</v>
       </c>
-      <c r="G41" s="258">
+      <c r="H41" s="258">
         <v>0.41</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="50.25" thickBot="1">
+    <row r="42" spans="1:8" ht="50.25" thickBot="1">
       <c r="A42" s="267" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="258" t="s">
+      <c r="B42" s="268"/>
+      <c r="C42" s="258" t="s">
         <v>567</v>
       </c>
-      <c r="C42" s="258">
+      <c r="D42" s="258">
         <v>1.2</v>
       </c>
-      <c r="D42" s="268">
+      <c r="E42" s="268">
         <v>0.47</v>
       </c>
-      <c r="E42" s="268">
+      <c r="F42" s="268">
         <v>0.12</v>
       </c>
-      <c r="F42" s="258">
+      <c r="G42" s="258">
         <v>1.67</v>
       </c>
-      <c r="G42" s="258">
+      <c r="H42" s="258">
         <v>0.12</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="50.25" thickBot="1">
+    <row r="43" spans="1:8" ht="50.25" thickBot="1">
       <c r="A43" s="267" t="s">
         <v>349</v>
       </c>
-      <c r="B43" s="258" t="s">
+      <c r="B43" s="268"/>
+      <c r="C43" s="258" t="s">
         <v>567</v>
       </c>
-      <c r="C43" s="258">
+      <c r="D43" s="258">
         <v>0.75</v>
       </c>
-      <c r="D43" s="268">
+      <c r="E43" s="268">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E43" s="268">
+      <c r="F43" s="268">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F43" s="258">
+      <c r="G43" s="258">
         <v>0.75</v>
       </c>
-      <c r="G43" s="258">
+      <c r="H43" s="258">
         <v>0.08</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.25" thickBot="1">
+    <row r="44" spans="1:8" ht="17.25" thickBot="1">
       <c r="A44" s="267" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="258" t="s">
+      <c r="B44" s="268"/>
+      <c r="C44" s="258" t="s">
         <v>567</v>
       </c>
-      <c r="C44" s="258">
+      <c r="D44" s="258">
         <v>0.06</v>
       </c>
-      <c r="D44" s="258">
+      <c r="E44" s="258">
         <v>0.04</v>
       </c>
-      <c r="E44" s="258">
+      <c r="F44" s="258">
         <v>0.01</v>
       </c>
-      <c r="F44" s="258">
+      <c r="G44" s="258">
         <v>0.16</v>
       </c>
-      <c r="G44" s="258">
+      <c r="H44" s="258">
         <v>0.13</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A45" s="274" t="s">
+    <row r="45" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A45" s="289" t="s">
         <v>526</v>
       </c>
-      <c r="B45" s="276"/>
-      <c r="C45" s="258">
-        <f>SUM(C33:C44)</f>
-        <v>9.1</v>
-      </c>
+      <c r="B45" s="301"/>
+      <c r="C45" s="291"/>
       <c r="D45" s="258">
         <f>SUM(D33:D44)</f>
-        <v>5.9700000000000006</v>
+        <v>9.1</v>
       </c>
       <c r="E45" s="258">
         <f>SUM(E33:E44)</f>
-        <v>3.6275000000000004</v>
+        <v>5.9700000000000006</v>
       </c>
       <c r="F45" s="258">
         <f>SUM(F33:F44)</f>
-        <v>15.800000000000002</v>
+        <v>3.6275000000000004</v>
       </c>
       <c r="G45" s="258">
         <f>SUM(G33:G44)</f>
+        <v>15.800000000000002</v>
+      </c>
+      <c r="H45" s="258">
+        <f>SUM(H33:H44)</f>
         <v>1.42</v>
       </c>
     </row>
+    <row r="50" spans="1:14" ht="13.5" thickBot="1"/>
+    <row r="51" spans="1:14" ht="50.25" thickBot="1">
+      <c r="A51" s="303"/>
+      <c r="B51" s="303" t="s">
+        <v>582</v>
+      </c>
+      <c r="C51" s="303" t="s">
+        <v>578</v>
+      </c>
+      <c r="D51" s="303" t="s">
+        <v>579</v>
+      </c>
+      <c r="E51" s="303" t="s">
+        <v>568</v>
+      </c>
+      <c r="F51" s="303" t="s">
+        <v>580</v>
+      </c>
+      <c r="G51" s="304" t="s">
+        <v>581</v>
+      </c>
+      <c r="I51" s="315" t="s">
+        <v>525</v>
+      </c>
+      <c r="J51" s="316" t="s">
+        <v>575</v>
+      </c>
+      <c r="K51" s="316" t="s">
+        <v>137</v>
+      </c>
+      <c r="L51" s="316" t="s">
+        <v>134</v>
+      </c>
+      <c r="M51" s="316" t="s">
+        <v>497</v>
+      </c>
+      <c r="N51" s="316" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="17.25" thickBot="1">
+      <c r="A52" s="305" t="s">
+        <v>577</v>
+      </c>
+      <c r="B52" s="260">
+        <v>16</v>
+      </c>
+      <c r="C52" s="303">
+        <v>10</v>
+      </c>
+      <c r="D52" s="303">
+        <v>2</v>
+      </c>
+      <c r="E52" s="303">
+        <v>4</v>
+      </c>
+      <c r="F52" s="303">
+        <v>0</v>
+      </c>
+      <c r="G52" s="306">
+        <v>0</v>
+      </c>
+      <c r="I52" s="274" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" s="258">
+        <v>1</v>
+      </c>
+      <c r="K52" s="258">
+        <v>1</v>
+      </c>
+      <c r="L52" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="M52" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N52" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="33.75" thickBot="1">
+      <c r="A53" s="305"/>
+      <c r="B53" s="309">
+        <v>1</v>
+      </c>
+      <c r="C53" s="303">
+        <v>62.5</v>
+      </c>
+      <c r="D53" s="303">
+        <v>12.5</v>
+      </c>
+      <c r="E53" s="303">
+        <v>25</v>
+      </c>
+      <c r="F53" s="303">
+        <v>0</v>
+      </c>
+      <c r="G53" s="306"/>
+      <c r="I53" s="274" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="258">
+        <v>21</v>
+      </c>
+      <c r="K53" s="258">
+        <v>20</v>
+      </c>
+      <c r="L53" s="258">
+        <v>1</v>
+      </c>
+      <c r="M53" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N53" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="17.25" thickBot="1">
+      <c r="A54" s="302"/>
+      <c r="B54" s="302"/>
+      <c r="I54" s="274" t="s">
+        <v>27</v>
+      </c>
+      <c r="J54" s="258">
+        <v>7</v>
+      </c>
+      <c r="K54" s="258">
+        <v>6</v>
+      </c>
+      <c r="L54" s="258">
+        <v>1</v>
+      </c>
+      <c r="M54" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N54" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="17.25" thickBot="1">
+      <c r="I55" s="274" t="s">
+        <v>43</v>
+      </c>
+      <c r="J55" s="258">
+        <v>1</v>
+      </c>
+      <c r="K55" s="258">
+        <v>0</v>
+      </c>
+      <c r="L55" s="258">
+        <v>1</v>
+      </c>
+      <c r="M55" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N55" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="17.25" thickBot="1">
+      <c r="I56" s="274" t="s">
+        <v>61</v>
+      </c>
+      <c r="J56" s="258">
+        <v>2</v>
+      </c>
+      <c r="K56" s="258">
+        <v>2</v>
+      </c>
+      <c r="L56" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="M56" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N56" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="33.75" thickBot="1">
+      <c r="I57" s="274" t="s">
+        <v>66</v>
+      </c>
+      <c r="J57" s="258">
+        <v>3</v>
+      </c>
+      <c r="K57" s="258">
+        <v>2</v>
+      </c>
+      <c r="L57" s="258">
+        <v>1</v>
+      </c>
+      <c r="M57" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N57" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="33.75" thickBot="1">
+      <c r="I58" s="274" t="s">
+        <v>77</v>
+      </c>
+      <c r="J58" s="258">
+        <v>3</v>
+      </c>
+      <c r="K58" s="258">
+        <v>3</v>
+      </c>
+      <c r="L58" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="M58" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N58" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="33.75" thickBot="1">
+      <c r="I59" s="274" t="s">
+        <v>85</v>
+      </c>
+      <c r="J59" s="258">
+        <v>4</v>
+      </c>
+      <c r="K59" s="258">
+        <v>3</v>
+      </c>
+      <c r="L59" s="258">
+        <v>1</v>
+      </c>
+      <c r="M59" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N59" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="33.75" thickBot="1">
+      <c r="I60" s="274" t="s">
+        <v>569</v>
+      </c>
+      <c r="J60" s="258">
+        <v>49</v>
+      </c>
+      <c r="K60" s="258">
+        <v>49</v>
+      </c>
+      <c r="L60" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="M60" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N60" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="50.25" thickBot="1">
+      <c r="I61" s="274" t="s">
+        <v>104</v>
+      </c>
+      <c r="J61" s="258">
+        <v>7</v>
+      </c>
+      <c r="K61" s="258">
+        <v>7</v>
+      </c>
+      <c r="L61" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="M61" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N61" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="50.25" thickBot="1">
+      <c r="I62" s="274" t="s">
+        <v>349</v>
+      </c>
+      <c r="J62" s="258">
+        <v>4</v>
+      </c>
+      <c r="K62" s="258">
+        <v>4</v>
+      </c>
+      <c r="L62" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="M62" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N62" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="17.25" thickBot="1">
+      <c r="I63" s="274" t="s">
+        <v>115</v>
+      </c>
+      <c r="J63" s="258">
+        <v>1</v>
+      </c>
+      <c r="K63" s="258">
+        <v>1</v>
+      </c>
+      <c r="L63" s="258">
+        <v>0</v>
+      </c>
+      <c r="M63" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N63" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="17.25" thickBot="1">
+      <c r="I64" s="274" t="s">
+        <v>526</v>
+      </c>
+      <c r="J64" s="258">
+        <f>SUM(J52:J63)</f>
+        <v>103</v>
+      </c>
+      <c r="K64" s="258">
+        <f>SUM(K52:K63)</f>
+        <v>98</v>
+      </c>
+      <c r="L64" s="258">
+        <v>5</v>
+      </c>
+      <c r="M64" s="258" t="s">
+        <v>576</v>
+      </c>
+      <c r="N64" s="258" t="s">
+        <v>576</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A13"/>
     <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A52:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D0CB1E-971C-4217-B4F0-2CE6B9DF7A16}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C10" sqref="C9:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A1" s="310"/>
+      <c r="B1" s="311" t="s">
+        <v>583</v>
+      </c>
+      <c r="C1" s="311" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="311" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="141" thickBot="1">
+      <c r="A2" s="312">
+        <v>1</v>
+      </c>
+      <c r="B2" s="313" t="s">
+        <v>584</v>
+      </c>
+      <c r="C2" s="314" t="s">
+        <v>589</v>
+      </c>
+      <c r="D2" s="317" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="153.75" thickBot="1">
+      <c r="A3" s="312">
+        <v>2</v>
+      </c>
+      <c r="B3" s="313" t="s">
+        <v>586</v>
+      </c>
+      <c r="C3" s="314" t="s">
+        <v>588</v>
+      </c>
+      <c r="D3" s="317" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="141" thickBot="1">
+      <c r="A4" s="312">
+        <v>3</v>
+      </c>
+      <c r="B4" s="313" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="314" t="s">
+        <v>590</v>
+      </c>
+      <c r="D4" s="317" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="166.5" thickBot="1">
+      <c r="A5" s="312">
+        <v>4</v>
+      </c>
+      <c r="B5" s="313" t="s">
+        <v>591</v>
+      </c>
+      <c r="C5" s="314" t="s">
+        <v>592</v>
+      </c>
+      <c r="D5" s="317" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="166.5" thickBot="1">
+      <c r="A6" s="312">
+        <v>5</v>
+      </c>
+      <c r="B6" s="313" t="s">
+        <v>587</v>
+      </c>
+      <c r="C6" s="314" t="s">
+        <v>593</v>
+      </c>
+      <c r="D6" s="317" t="s">
+        <v>568</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>